<commit_message>
Add new meeting notes and update availability
</commit_message>
<xml_diff>
--- a/Organisation/Availability.xlsx
+++ b/Organisation/Availability.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ostch-my.sharepoint.com/personal/benjamin_plattner_ost_ch/Documents/KubeWatch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnz\dev-workspace\kubewatch\Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="8_{4EB3E691-A84B-477E-832C-60651BC00E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C33B2750-F597-4725-BF03-2C5B8C9F979E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34355961-853D-46D5-A6D2-4594BB629E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2DB7FBEC-5C61-4DC1-9E47-FC23E1BC465B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15394" xr2:uid="{2DB7FBEC-5C61-4DC1-9E47-FC23E1BC465B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,6 +405,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,10 +418,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,75 +898,75 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="51" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="51" width="2.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="18" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
-      <c r="AY1" s="20"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="24"/>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="K3" s="6">
         <v>3</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3" s="20">
         <v>3</v>
       </c>
       <c r="M3" s="5">
@@ -1185,7 +1185,7 @@
       <c r="U3" s="6">
         <v>3</v>
       </c>
-      <c r="V3" s="23">
+      <c r="V3" s="20">
         <v>3</v>
       </c>
       <c r="W3" s="5">
@@ -1215,7 +1215,7 @@
       <c r="AE3" s="6">
         <v>1</v>
       </c>
-      <c r="AF3" s="23">
+      <c r="AF3" s="20">
         <v>1</v>
       </c>
       <c r="AG3" s="5">
@@ -1245,7 +1245,7 @@
       <c r="AO3" s="6">
         <v>1</v>
       </c>
-      <c r="AP3" s="23">
+      <c r="AP3" s="20">
         <v>3</v>
       </c>
       <c r="AQ3" s="5">
@@ -1276,15 +1276,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
       <c r="C4" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="15">
         <v>3</v>
@@ -1310,7 +1310,7 @@
       <c r="K4" s="8">
         <v>3</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="21">
         <v>3</v>
       </c>
       <c r="M4" s="7">
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="7">
         <v>3</v>
@@ -1340,7 +1340,7 @@
       <c r="U4" s="8">
         <v>1</v>
       </c>
-      <c r="V4" s="24">
+      <c r="V4" s="21">
         <v>3</v>
       </c>
       <c r="W4" s="7">
@@ -1370,7 +1370,7 @@
       <c r="AE4" s="8">
         <v>1</v>
       </c>
-      <c r="AF4" s="24">
+      <c r="AF4" s="21">
         <v>1</v>
       </c>
       <c r="AG4" s="7">
@@ -1400,7 +1400,7 @@
       <c r="AO4" s="8">
         <v>1</v>
       </c>
-      <c r="AP4" s="24">
+      <c r="AP4" s="21">
         <v>3</v>
       </c>
       <c r="AQ4" s="7">
@@ -1431,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -1465,7 +1465,7 @@
       <c r="K5" s="8">
         <v>3</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="21">
         <v>2</v>
       </c>
       <c r="M5" s="7">
@@ -1478,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="7">
         <v>1</v>
@@ -1495,7 +1495,7 @@
       <c r="U5" s="8">
         <v>2</v>
       </c>
-      <c r="V5" s="24">
+      <c r="V5" s="21">
         <v>3</v>
       </c>
       <c r="W5" s="7">
@@ -1525,7 +1525,7 @@
       <c r="AE5" s="8">
         <v>2</v>
       </c>
-      <c r="AF5" s="24">
+      <c r="AF5" s="21">
         <v>3</v>
       </c>
       <c r="AG5" s="7">
@@ -1555,7 +1555,7 @@
       <c r="AO5" s="8">
         <v>2</v>
       </c>
-      <c r="AP5" s="24">
+      <c r="AP5" s="21">
         <v>3</v>
       </c>
       <c r="AQ5" s="7">
@@ -1586,15 +1586,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>2</v>
       </c>
       <c r="C6" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7">
         <v>3</v>
@@ -1620,7 +1620,7 @@
       <c r="K6" s="8">
         <v>3</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="20">
         <v>3</v>
       </c>
       <c r="M6" s="5">
@@ -1633,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="17">
         <v>2</v>
@@ -1650,7 +1650,7 @@
       <c r="U6" s="8">
         <v>3</v>
       </c>
-      <c r="V6" s="24">
+      <c r="V6" s="21">
         <v>3</v>
       </c>
       <c r="W6" s="7">
@@ -1680,7 +1680,7 @@
       <c r="AE6" s="8">
         <v>3</v>
       </c>
-      <c r="AF6" s="24">
+      <c r="AF6" s="21">
         <v>1</v>
       </c>
       <c r="AG6" s="7">
@@ -1710,7 +1710,7 @@
       <c r="AO6" s="8">
         <v>1</v>
       </c>
-      <c r="AP6" s="24">
+      <c r="AP6" s="21">
         <v>1</v>
       </c>
       <c r="AQ6" s="7">
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>

</xml_diff>